<commit_message>
archivos excels y bd actualizados
</commit_message>
<xml_diff>
--- a/Archivos/Excel/Equipos.xlsx
+++ b/Archivos/Excel/Equipos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\velve\Documents\ProyectosVisual\1-Projectos de Java\Archivos\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E7621C-9EA6-44BE-8E0A-F49C16E61850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C11823-7887-4C3B-B907-5A01C37133F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>CodiHospi</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>idEquipo</t>
+  </si>
+  <si>
+    <t>2020-11-09  20:30:20</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +584,70 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4000</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2800</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>